<commit_message>
Have a plot for each of 3 separate processes
</commit_message>
<xml_diff>
--- a/Part BProcess 491 2500Datasample scatter.xlsx
+++ b/Part BProcess 491 2500Datasample scatter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CS BU\CS 550 OS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josep\AppData\Local\Packages\CanonicalGroupLimited.UbuntuonWindows_79rhkp1fndgsc\LocalState\rootfs\root\cs550\assignment3DONOTRUNLOCALLY\CS550Assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C83FE786-44DB-4375-B0CC-0F19D53164E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDCE213-1825-44F4-B872-7B4936E996D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A457CB97-E8BC-44B7-A7E9-80C74E57CE7A}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Planted</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>&gt;&gt;time elapsed in seconds</t>
+  </si>
+  <si>
+    <t>120 data points</t>
+  </si>
+  <si>
+    <t>2300 data points</t>
   </si>
 </sst>
 </file>
@@ -134,6 +140,36 @@
   <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Over</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 2300 Data points process 491 systemd-journal</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14427,7 +14463,1077 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>120</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> data points process 491 systemd-journal</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$A$120</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="120"/>
+                <c:pt idx="0">
+                  <c:v>277702.26892599999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>277702.26892900001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>277702.26895699999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>277702.26896199997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>277702.26896999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>277702.26898400002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>277702.26898699999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>277702.26899000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>277702.26909999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>277702.26910799998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>277702.26912200003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>277702.26913500001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>277702.26913799997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>277702.26916800003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>277702.26917799999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>277702.26919700002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>277702.26920500002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>277702.26923500001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>277702.26924200001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>277702.26925100002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>277702.26926899998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>277702.26927699998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>277702.26930799999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>277702.26931100001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>277702.26931599999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>277702.26931800001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>277702.26934100001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>277702.26936799998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>277702.26937599998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>277702.26940300001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>277702.26941100002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>277702.26943400002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>277702.26943699998</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>277702.26945800002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>277702.269462</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>277702.26946600003</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>277702.26948800002</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>277702.26949699997</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>277702.269524</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>277702.26953200001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>277702.26955999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>277702.26956300001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>277702.26958700002</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>277702.26959099999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>277702.26961199997</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>277702.26962400001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>277702.26962699997</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>277702.26964999997</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>277702.269654</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>277702.26965700003</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>277702.269677</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>277702.26968099998</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>277702.26970599999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>277702.26971299999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>277702.26973499998</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>277702.26973900001</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>277702.269761</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>277702.26976499998</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>277702.269791</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>277702.26979799999</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>277702.26982599997</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>277702.26982799999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>277702.26983200002</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>277702.26985500002</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>277702.26986200002</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>277702.26986900001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>277702.26989599998</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>277702.26990000001</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>277702.26992599998</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>277702.26993399998</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>277702.26996100001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>277702.26996399998</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>277702.26997099997</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>277702.26999399997</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>277702.27000199998</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>277702.27002900001</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>277702.270036</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>277702.27006499999</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>277702.27008799999</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>277702.27011400001</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>277702.27011799999</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>277702.27014600002</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>277702.27016800002</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>277702.27017799998</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>277702.270181</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>277702.27019900002</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>277702.27020799997</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>277702.27021400002</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>277702.27023600001</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>277702.27024400001</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>277702.27027099999</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>277702.27027500002</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>277702.27029700001</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>277702.27032299998</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>277702.27033099998</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>277702.270357</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>277702.27036099997</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>277702.27038300002</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>277702.27039700001</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>277702.27041499998</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>277702.270441</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>277702.27045000001</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>277702.27045200003</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>277702.270456</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>277702.270479</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>277702.27048299997</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>277702.27050799999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>277702.27051100001</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>277702.27053400001</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>277702.27054100001</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>277702.27056700003</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>277702.27058399998</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>277702.27060500003</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>277702.270609</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>277702.27063099999</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>277702.27063599997</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>277702.27063799999</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>277702.27065999998</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>277702.27066699998</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>277702.27067400003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$120</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="120"/>
+                <c:pt idx="0">
+                  <c:v>140096514643576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>140096612050024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140096529158568</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>140096529621824</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>140096530076744</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>140096513523064</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>140096616407936</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140096545077280</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>140096518529024</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>140096614191904</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>140096614457920</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>140096548814336</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140096615328696</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140096614004864</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140096517726216</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>140096612224992</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>140096614749472</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>140096519709696</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>140096612171080</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>140096518524088</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>140096614833776</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>140096613917104</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>140096564301328</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>140096613698872</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>140096563935376</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>140096614800792</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>140096612439104</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140096614429248</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>140096614168464</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>140096614438224</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>140096613240640</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>140096611892208</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>140096611877008</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>140096611619824</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>140096611966352</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>140096518533120</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>140096612029040</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>140096613651616</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>140096614595408</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>140096614224464</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>140096517101200</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>140096614513720</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>140096612298224</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>140096611666192</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>140096611816832</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>140096546715096</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>140096612797096</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>140096611797296</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>140096561331968</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>140096614945592</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>140096615040784</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>140096611995616</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>140096614529744</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>140096613669472</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>140096611907312</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>140096615157712</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>140096612157456</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>140096518537216</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>140096613840816</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>140096614622112</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>140096547990360</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>140096612864232</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>140096615069120</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>140096515114176</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>140096613876568</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>140096612856624</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>140096612804032</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>140096612481616</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>140096613784576</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>140096614754336</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>140096555574464</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>140096613817016</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>140096613357088</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>140096615029936</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>140096613124672</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>140096614384960</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>140096614443120</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>140096613500032</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>140096612072800</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>140096518541312</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>140096614648080</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>140096613850512</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>140096519358904</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>140096615235728</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>140096536396552</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>140096614924912</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>140096530525504</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>140096614252920</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>140096615015712</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>140096613018080</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>140096614645664</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>140096614787568</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>140096611565760</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>140096614687136</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>140096612770352</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>140096613030576</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>140096612509552</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>140096612228464</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>140096517725016</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>140096615026240</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>140096613927472</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>140096536628808</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>140096613723944</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>140096518545416</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>140096614959968</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>140096612217808</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>140096614633472</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>140096615049792</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>140096611637376</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>140096614462976</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>140096614228544</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>140096517733816</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>140096613710224</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>140096615219696</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>140096613907248</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>140096536163576</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>140096611584664</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>140096564133832</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>140096615098936</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>140096614583856</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-444D-4AC0-955C-AC0ECE657E59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="489042808"/>
+        <c:axId val="489043464"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="489042808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="489043464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="489043464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="489042808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -14983,6 +16089,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -15018,6 +16640,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F990A4C-177C-4023-9734-7602DAE8848C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -15613,10 +17271,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D436D83B-7E4F-4D9D-A42A-75CBB2FD96C2}">
-  <dimension ref="A1:J2338"/>
+  <dimension ref="A1:Q2338"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15628,7 +17286,7 @@
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>277702.26892599999</v>
       </c>
@@ -15651,7 +17309,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>277702.26892900001</v>
       </c>
@@ -15659,7 +17317,7 @@
         <v>140096612050024</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>277702.26895699999</v>
       </c>
@@ -15674,7 +17332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>277702.26896199997</v>
       </c>
@@ -15682,15 +17340,21 @@
         <v>140096529621824</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>277702.26896999998</v>
       </c>
       <c r="B5" s="1">
         <v>140096530076744</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>277702.26898400002</v>
       </c>
@@ -15698,7 +17362,7 @@
         <v>140096513523064</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>277702.26898699999</v>
       </c>
@@ -15706,7 +17370,7 @@
         <v>140096616407936</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>277702.26899000001</v>
       </c>
@@ -15714,7 +17378,7 @@
         <v>140096545077280</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>277702.26909999998</v>
       </c>
@@ -15722,7 +17386,7 @@
         <v>140096518529024</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>277702.26910799998</v>
       </c>
@@ -15730,7 +17394,7 @@
         <v>140096614191904</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>277702.26912200003</v>
       </c>
@@ -15738,7 +17402,7 @@
         <v>140096614457920</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>277702.26913500001</v>
       </c>
@@ -15746,7 +17410,7 @@
         <v>140096548814336</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>277702.26913799997</v>
       </c>
@@ -15754,7 +17418,7 @@
         <v>140096615328696</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>277702.26916800003</v>
       </c>
@@ -15762,7 +17426,7 @@
         <v>140096614004864</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>277702.26917799999</v>
       </c>
@@ -15770,7 +17434,7 @@
         <v>140096517726216</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>277702.26919700002</v>
       </c>

</xml_diff>